<commit_message>
Oops, labels swapped (thanks Jordan)
</commit_message>
<xml_diff>
--- a/Data/02_TimeData/CommunicationTechnologyEnergyUse.xlsx
+++ b/Data/02_TimeData/CommunicationTechnologyEnergyUse.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="460" windowWidth="32500" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>Best case, with gains in energy efficiency</t>
   </si>
   <si>
-    <t>Expected case, without gains in energy effiency</t>
-  </si>
-  <si>
-    <t>Expected case, with in energy efficiency</t>
-  </si>
-  <si>
     <t>Communication Technology Share of Total Global Electricity Usage</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>Best case (with gains in energy efficiency), in terawatts per hour (TWh)</t>
+  </si>
+  <si>
+    <t>Expected case, without gains in energy efficiency</t>
+  </si>
+  <si>
+    <t>Expected case, with gains in energy effiency</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A2:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -525,7 +525,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>1743.8964456078272</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>1743.8964456078272</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>2015</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>2015</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1">
         <v>2010</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5">
         <v>8.2343156786699012E-2</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5">
         <v>7.8346574927402726E-2</v>
@@ -1018,27 +1018,27 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>